<commit_message>
Deploying to gh-pages from  @ 6e453d78d44633b99ca6b6f44e7d70e253104cc2 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2025_4-1-5.xlsx
+++ b/assets/excel/2025_4-1-5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15_Uebergreifende_Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3668A234-DAD1-4A6B-B686-A19219CF0790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1477E6FD-6052-44B2-A6C7-8985E9737F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{25B46B2B-FF1A-413B-AD77-D797683F7C16}"/>
   </bookViews>
@@ -421,42 +421,18 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -506,6 +482,30 @@
     </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -827,11 +827,13 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
@@ -864,1266 +866,1266 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="6" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B6" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11" t="s">
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+    </row>
+    <row r="7" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B7" s="30"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11" t="s">
+      <c r="F7" s="36"/>
+      <c r="G7" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="2:10" s="7" customFormat="1" ht="41.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10" t="s">
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+    </row>
+    <row r="8" spans="2:10" s="4" customFormat="1" ht="41.25">
+      <c r="B8" s="30"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="12" t="s">
+    <row r="9" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B9" s="31"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B10" s="17">
+    <row r="10" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B10" s="9">
         <v>1</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="10">
         <v>2</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="10">
         <v>3</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="10">
         <v>4</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="10">
         <v>5</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="10">
         <v>6</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="10">
         <v>7</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="10">
         <v>8</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B11" s="32">
+    <row r="11" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B11" s="24">
         <v>2024</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="25">
         <v>579</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="25">
         <v>4224</v>
       </c>
-      <c r="G11" s="33">
+      <c r="G11" s="25">
         <v>81</v>
       </c>
-      <c r="H11" s="33">
+      <c r="H11" s="25">
         <v>737</v>
       </c>
-      <c r="I11" s="34">
+      <c r="I11" s="26">
         <v>14</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="26">
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="12" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B12" s="32">
+    <row r="12" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B12" s="24">
         <v>2024</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="25">
         <v>298</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="25">
         <v>2122</v>
       </c>
-      <c r="G12" s="33">
+      <c r="G12" s="25">
         <v>50</v>
       </c>
-      <c r="H12" s="33">
+      <c r="H12" s="25">
         <v>368</v>
       </c>
-      <c r="I12" s="34">
+      <c r="I12" s="26">
         <v>16.8</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12" s="26">
         <v>17.3</v>
       </c>
     </row>
-    <row r="13" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B13" s="32">
+    <row r="13" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B13" s="24">
         <v>2024</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="25">
         <v>282</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="25">
         <v>2103</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="25">
         <v>31</v>
       </c>
-      <c r="H13" s="33">
+      <c r="H13" s="25">
         <v>369</v>
       </c>
-      <c r="I13" s="34">
+      <c r="I13" s="26">
         <v>11</v>
       </c>
-      <c r="J13" s="34">
+      <c r="J13" s="26">
         <v>17.5</v>
       </c>
     </row>
-    <row r="14" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B14" s="32">
+    <row r="14" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B14" s="24">
         <v>2024</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="25">
         <v>387</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="25">
         <v>3107</v>
       </c>
-      <c r="G14" s="33">
+      <c r="G14" s="25">
         <v>38</v>
       </c>
-      <c r="H14" s="33">
+      <c r="H14" s="25">
         <v>341</v>
       </c>
-      <c r="I14" s="34">
+      <c r="I14" s="26">
         <v>9.8000000000000007</v>
       </c>
-      <c r="J14" s="34">
+      <c r="J14" s="26">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B15" s="32">
+    <row r="15" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B15" s="24">
         <v>2024</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E15" s="25">
         <v>195</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="25">
         <v>1561</v>
       </c>
-      <c r="G15" s="33">
+      <c r="G15" s="25">
         <v>24</v>
       </c>
-      <c r="H15" s="33">
+      <c r="H15" s="25">
         <v>161</v>
       </c>
-      <c r="I15" s="34">
+      <c r="I15" s="26">
         <v>12</v>
       </c>
-      <c r="J15" s="34">
+      <c r="J15" s="26">
         <v>10.3</v>
       </c>
     </row>
-    <row r="16" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B16" s="32">
+    <row r="16" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B16" s="24">
         <v>2024</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E16" s="25">
         <v>191</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="25">
         <v>1546</v>
       </c>
-      <c r="G16" s="33">
+      <c r="G16" s="25">
         <v>15</v>
       </c>
-      <c r="H16" s="33">
+      <c r="H16" s="25">
         <v>180</v>
       </c>
-      <c r="I16" s="34">
+      <c r="I16" s="26">
         <v>7.6</v>
       </c>
-      <c r="J16" s="34">
+      <c r="J16" s="26">
         <v>11.6</v>
       </c>
     </row>
-    <row r="17" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B17" s="32">
+    <row r="17" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B17" s="24">
         <v>2024</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="25">
         <v>192</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="25">
         <v>1117</v>
       </c>
-      <c r="G17" s="33">
+      <c r="G17" s="25">
         <v>43</v>
       </c>
-      <c r="H17" s="33">
+      <c r="H17" s="25">
         <v>396</v>
       </c>
-      <c r="I17" s="34">
+      <c r="I17" s="26">
         <v>22.3</v>
       </c>
-      <c r="J17" s="34">
+      <c r="J17" s="26">
         <v>35.4</v>
       </c>
     </row>
-    <row r="18" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B18" s="32">
+    <row r="18" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B18" s="24">
         <v>2024</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E18" s="25">
         <v>102</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="25">
         <v>561</v>
       </c>
-      <c r="G18" s="33">
+      <c r="G18" s="25">
         <v>27</v>
       </c>
-      <c r="H18" s="33">
+      <c r="H18" s="25">
         <v>207</v>
       </c>
-      <c r="I18" s="34">
+      <c r="I18" s="26">
         <v>26</v>
       </c>
-      <c r="J18" s="34">
+      <c r="J18" s="26">
         <v>36.9</v>
       </c>
     </row>
-    <row r="19" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B19" s="32">
+    <row r="19" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B19" s="24">
         <v>2024</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="25">
         <v>90</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="25">
         <v>557</v>
       </c>
-      <c r="G19" s="33">
+      <c r="G19" s="25">
         <v>16</v>
       </c>
-      <c r="H19" s="33">
+      <c r="H19" s="25">
         <v>189</v>
       </c>
-      <c r="I19" s="34">
+      <c r="I19" s="26">
         <v>18.100000000000001</v>
       </c>
-      <c r="J19" s="34">
+      <c r="J19" s="26">
         <v>33.9</v>
       </c>
     </row>
-    <row r="20" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B20" s="35">
+    <row r="20" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B20" s="27">
         <v>2023</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="25">
         <v>594</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="25">
         <v>4227</v>
       </c>
-      <c r="G20" s="33">
+      <c r="G20" s="25">
         <v>85</v>
       </c>
-      <c r="H20" s="33">
+      <c r="H20" s="25">
         <v>781</v>
       </c>
-      <c r="I20" s="34">
+      <c r="I20" s="26">
         <v>14.3</v>
       </c>
-      <c r="J20" s="34">
+      <c r="J20" s="26">
         <v>18.5</v>
       </c>
     </row>
-    <row r="21" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B21" s="35">
+    <row r="21" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B21" s="27">
         <v>2023</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="25">
         <v>301</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="25">
         <v>2121</v>
       </c>
-      <c r="G21" s="33">
+      <c r="G21" s="25">
         <v>51</v>
       </c>
-      <c r="H21" s="33">
+      <c r="H21" s="25">
         <v>386</v>
       </c>
-      <c r="I21" s="34">
+      <c r="I21" s="26">
         <v>17</v>
       </c>
-      <c r="J21" s="34">
+      <c r="J21" s="26">
         <v>18.2</v>
       </c>
     </row>
-    <row r="22" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B22" s="35">
+    <row r="22" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B22" s="27">
         <v>2023</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="25">
         <v>292</v>
       </c>
-      <c r="F22" s="33">
+      <c r="F22" s="25">
         <v>2106</v>
       </c>
-      <c r="G22" s="33">
+      <c r="G22" s="25">
         <v>34</v>
       </c>
-      <c r="H22" s="33">
+      <c r="H22" s="25">
         <v>394</v>
       </c>
-      <c r="I22" s="34">
+      <c r="I22" s="26">
         <v>11.6</v>
       </c>
-      <c r="J22" s="34">
+      <c r="J22" s="26">
         <v>18.7</v>
       </c>
     </row>
-    <row r="23" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B23" s="35">
+    <row r="23" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B23" s="27">
         <v>2023</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E23" s="25">
         <v>405</v>
       </c>
-      <c r="F23" s="33">
+      <c r="F23" s="25">
         <v>3161</v>
       </c>
-      <c r="G23" s="33">
+      <c r="G23" s="25">
         <v>42</v>
       </c>
-      <c r="H23" s="33">
+      <c r="H23" s="25">
         <v>390</v>
       </c>
-      <c r="I23" s="34">
+      <c r="I23" s="26">
         <v>10.3</v>
       </c>
-      <c r="J23" s="34">
+      <c r="J23" s="26">
         <v>12.3</v>
       </c>
     </row>
-    <row r="24" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B24" s="35">
+    <row r="24" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B24" s="27">
         <v>2023</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="33">
+      <c r="E24" s="25">
         <v>203</v>
       </c>
-      <c r="F24" s="33">
+      <c r="F24" s="25">
         <v>1580</v>
       </c>
-      <c r="G24" s="33">
+      <c r="G24" s="25">
         <v>23</v>
       </c>
-      <c r="H24" s="33">
+      <c r="H24" s="25">
         <v>183</v>
       </c>
-      <c r="I24" s="34">
+      <c r="I24" s="26">
         <v>11.3</v>
       </c>
-      <c r="J24" s="34">
+      <c r="J24" s="26">
         <v>11.6</v>
       </c>
     </row>
-    <row r="25" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B25" s="35">
+    <row r="25" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B25" s="27">
         <v>2023</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="25">
         <v>202</v>
       </c>
-      <c r="F25" s="33">
+      <c r="F25" s="25">
         <v>1581</v>
       </c>
-      <c r="G25" s="33">
+      <c r="G25" s="25">
         <v>19</v>
       </c>
-      <c r="H25" s="33">
+      <c r="H25" s="25">
         <v>207</v>
       </c>
-      <c r="I25" s="34">
+      <c r="I25" s="26">
         <v>9.3000000000000007</v>
       </c>
-      <c r="J25" s="34">
+      <c r="J25" s="26">
         <v>13.1</v>
       </c>
     </row>
-    <row r="26" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B26" s="35">
+    <row r="26" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B26" s="27">
         <v>2023</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C26" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="33">
+      <c r="E26" s="25">
         <v>189</v>
       </c>
-      <c r="F26" s="33">
+      <c r="F26" s="25">
         <v>1066</v>
       </c>
-      <c r="G26" s="33">
+      <c r="G26" s="25">
         <v>43</v>
       </c>
-      <c r="H26" s="33">
+      <c r="H26" s="25">
         <v>391</v>
       </c>
-      <c r="I26" s="34">
+      <c r="I26" s="26">
         <v>23</v>
       </c>
-      <c r="J26" s="34">
+      <c r="J26" s="26">
         <v>36.700000000000003</v>
       </c>
     </row>
-    <row r="27" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B27" s="35">
+    <row r="27" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B27" s="27">
         <v>2023</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="C27" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="25">
         <v>98</v>
       </c>
-      <c r="F27" s="33">
+      <c r="F27" s="25">
         <v>541</v>
       </c>
-      <c r="G27" s="33">
+      <c r="G27" s="25">
         <v>28</v>
       </c>
-      <c r="H27" s="33">
+      <c r="H27" s="25">
         <v>203</v>
       </c>
-      <c r="I27" s="34">
+      <c r="I27" s="26">
         <v>28.9</v>
       </c>
-      <c r="J27" s="34">
+      <c r="J27" s="26">
         <v>37.6</v>
       </c>
     </row>
-    <row r="28" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B28" s="35">
+    <row r="28" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B28" s="27">
         <v>2023</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="C28" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="33">
+      <c r="E28" s="25">
         <v>91</v>
       </c>
-      <c r="F28" s="33">
+      <c r="F28" s="25">
         <v>525</v>
       </c>
-      <c r="G28" s="33">
+      <c r="G28" s="25">
         <v>15</v>
       </c>
-      <c r="H28" s="33">
+      <c r="H28" s="25">
         <v>188</v>
       </c>
-      <c r="I28" s="34">
+      <c r="I28" s="26">
         <v>16.600000000000001</v>
       </c>
-      <c r="J28" s="34">
+      <c r="J28" s="26">
         <v>35.799999999999997</v>
       </c>
     </row>
-    <row r="29" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B29" s="35">
+    <row r="29" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B29" s="27">
         <v>2022</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="33">
+      <c r="E29" s="25">
         <v>622</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="25">
         <v>4278</v>
       </c>
-      <c r="G29" s="33">
+      <c r="G29" s="25">
         <v>85</v>
       </c>
-      <c r="H29" s="33">
+      <c r="H29" s="25">
         <v>830</v>
       </c>
-      <c r="I29" s="34">
+      <c r="I29" s="26">
         <v>13.6</v>
       </c>
-      <c r="J29" s="34">
+      <c r="J29" s="26">
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="30" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B30" s="35">
+    <row r="30" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B30" s="27">
         <v>2022</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C30" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="33">
+      <c r="E30" s="25">
         <v>318</v>
       </c>
-      <c r="F30" s="33">
+      <c r="F30" s="25">
         <v>2142</v>
       </c>
-      <c r="G30" s="33">
+      <c r="G30" s="25">
         <v>48</v>
       </c>
-      <c r="H30" s="33">
+      <c r="H30" s="25">
         <v>413</v>
       </c>
-      <c r="I30" s="34">
+      <c r="I30" s="26">
         <v>15.2</v>
       </c>
-      <c r="J30" s="34">
+      <c r="J30" s="26">
         <v>19.3</v>
       </c>
     </row>
-    <row r="31" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B31" s="35">
+    <row r="31" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B31" s="27">
         <v>2022</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E31" s="33">
+      <c r="E31" s="25">
         <v>304</v>
       </c>
-      <c r="F31" s="33">
+      <c r="F31" s="25">
         <v>2136</v>
       </c>
-      <c r="G31" s="33">
+      <c r="G31" s="25">
         <v>37</v>
       </c>
-      <c r="H31" s="33">
+      <c r="H31" s="25">
         <v>417</v>
       </c>
-      <c r="I31" s="34">
+      <c r="I31" s="26">
         <v>12</v>
       </c>
-      <c r="J31" s="34">
+      <c r="J31" s="26">
         <v>19.5</v>
       </c>
     </row>
-    <row r="32" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B32" s="35">
+    <row r="32" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B32" s="27">
         <v>2022</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="33">
+      <c r="E32" s="25">
         <v>434</v>
       </c>
-      <c r="F32" s="33">
+      <c r="F32" s="25">
         <v>3195</v>
       </c>
-      <c r="G32" s="33">
+      <c r="G32" s="25">
         <v>43</v>
       </c>
-      <c r="H32" s="33">
+      <c r="H32" s="25">
         <v>427</v>
       </c>
-      <c r="I32" s="34">
+      <c r="I32" s="26">
         <v>9.8000000000000007</v>
       </c>
-      <c r="J32" s="34">
+      <c r="J32" s="26">
         <v>13.4</v>
       </c>
     </row>
-    <row r="33" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B33" s="35">
+    <row r="33" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B33" s="27">
         <v>2022</v>
       </c>
-      <c r="C33" s="33" t="s">
+      <c r="C33" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="33">
+      <c r="E33" s="25">
         <v>219</v>
       </c>
-      <c r="F33" s="33">
+      <c r="F33" s="25">
         <v>1592</v>
       </c>
-      <c r="G33" s="33">
+      <c r="G33" s="25">
         <v>22</v>
       </c>
-      <c r="H33" s="33">
+      <c r="H33" s="25">
         <v>202</v>
       </c>
-      <c r="I33" s="34">
+      <c r="I33" s="26">
         <v>10.1</v>
       </c>
-      <c r="J33" s="34">
+      <c r="J33" s="26">
         <v>12.7</v>
       </c>
     </row>
-    <row r="34" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B34" s="35">
+    <row r="34" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B34" s="27">
         <v>2022</v>
       </c>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E34" s="33">
+      <c r="E34" s="25">
         <v>215</v>
       </c>
-      <c r="F34" s="33">
+      <c r="F34" s="25">
         <v>1603</v>
       </c>
-      <c r="G34" s="33">
+      <c r="G34" s="25">
         <v>21</v>
       </c>
-      <c r="H34" s="33">
+      <c r="H34" s="25">
         <v>225</v>
       </c>
-      <c r="I34" s="34">
+      <c r="I34" s="26">
         <v>9.5</v>
       </c>
-      <c r="J34" s="34">
+      <c r="J34" s="26">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B35" s="35">
+    <row r="35" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B35" s="27">
         <v>2022</v>
       </c>
-      <c r="C35" s="33" t="s">
+      <c r="C35" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E35" s="33">
+      <c r="E35" s="25">
         <v>188</v>
       </c>
-      <c r="F35" s="33">
+      <c r="F35" s="25">
         <v>1083</v>
       </c>
-      <c r="G35" s="33">
+      <c r="G35" s="25">
         <v>42</v>
       </c>
-      <c r="H35" s="33">
+      <c r="H35" s="25">
         <v>403</v>
       </c>
-      <c r="I35" s="34">
+      <c r="I35" s="26">
         <v>22.5</v>
       </c>
-      <c r="J35" s="34">
+      <c r="J35" s="26">
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="36" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B36" s="35">
+    <row r="36" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B36" s="27">
         <v>2022</v>
       </c>
-      <c r="C36" s="33" t="s">
+      <c r="C36" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="33">
+      <c r="E36" s="25">
         <v>99</v>
       </c>
-      <c r="F36" s="33">
+      <c r="F36" s="25">
         <v>550</v>
       </c>
-      <c r="G36" s="33">
+      <c r="G36" s="25">
         <v>26</v>
       </c>
-      <c r="H36" s="33">
+      <c r="H36" s="25">
         <v>211</v>
       </c>
-      <c r="I36" s="34">
+      <c r="I36" s="26">
         <v>26.4</v>
       </c>
-      <c r="J36" s="34">
+      <c r="J36" s="26">
         <v>38.4</v>
       </c>
     </row>
-    <row r="37" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B37" s="35">
+    <row r="37" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B37" s="27">
         <v>2022</v>
       </c>
-      <c r="C37" s="33" t="s">
+      <c r="C37" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="33" t="s">
+      <c r="D37" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="33">
+      <c r="E37" s="25">
         <v>89</v>
       </c>
-      <c r="F37" s="33">
+      <c r="F37" s="25">
         <v>533</v>
       </c>
-      <c r="G37" s="33">
+      <c r="G37" s="25">
         <v>16</v>
       </c>
-      <c r="H37" s="33">
+      <c r="H37" s="25">
         <v>192</v>
       </c>
-      <c r="I37" s="34">
+      <c r="I37" s="26">
         <v>18.100000000000001</v>
       </c>
-      <c r="J37" s="34">
+      <c r="J37" s="26">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B38" s="35">
+    <row r="38" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B38" s="27">
         <v>2021</v>
       </c>
-      <c r="C38" s="33" t="s">
+      <c r="C38" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="33" t="s">
+      <c r="D38" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="33">
+      <c r="E38" s="25">
         <v>618</v>
       </c>
-      <c r="F38" s="33">
+      <c r="F38" s="25">
         <v>4254</v>
       </c>
-      <c r="G38" s="33">
+      <c r="G38" s="25">
         <v>79</v>
       </c>
-      <c r="H38" s="33">
+      <c r="H38" s="25">
         <v>815</v>
       </c>
-      <c r="I38" s="36" t="s">
+      <c r="I38" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="J38" s="36" t="s">
+      <c r="J38" s="28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B39" s="35">
+    <row r="39" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B39" s="27">
         <v>2021</v>
       </c>
-      <c r="C39" s="33" t="s">
+      <c r="C39" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D39" s="33" t="s">
+      <c r="D39" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="33">
+      <c r="E39" s="25">
         <v>318</v>
       </c>
-      <c r="F39" s="33">
+      <c r="F39" s="25">
         <v>2141</v>
       </c>
-      <c r="G39" s="33">
+      <c r="G39" s="25">
         <v>46</v>
       </c>
-      <c r="H39" s="33">
+      <c r="H39" s="25">
         <v>404</v>
       </c>
-      <c r="I39" s="36" t="s">
+      <c r="I39" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="J39" s="36" t="s">
+      <c r="J39" s="28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B40" s="35">
+    <row r="40" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B40" s="27">
         <v>2021</v>
       </c>
-      <c r="C40" s="33" t="s">
+      <c r="C40" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="33" t="s">
+      <c r="D40" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="33">
+      <c r="E40" s="25">
         <v>300</v>
       </c>
-      <c r="F40" s="33">
+      <c r="F40" s="25">
         <v>2113</v>
       </c>
-      <c r="G40" s="33">
+      <c r="G40" s="25">
         <v>34</v>
       </c>
-      <c r="H40" s="33">
+      <c r="H40" s="25">
         <v>411</v>
       </c>
-      <c r="I40" s="36" t="s">
+      <c r="I40" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="J40" s="36" t="s">
+      <c r="J40" s="28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B41" s="35">
+    <row r="41" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B41" s="27">
         <v>2021</v>
       </c>
-      <c r="C41" s="33" t="s">
+      <c r="C41" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="33" t="s">
+      <c r="D41" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E41" s="33">
+      <c r="E41" s="25">
         <v>434</v>
       </c>
-      <c r="F41" s="33">
+      <c r="F41" s="25">
         <v>3215</v>
       </c>
-      <c r="G41" s="33">
+      <c r="G41" s="25">
         <v>41</v>
       </c>
-      <c r="H41" s="33">
+      <c r="H41" s="25">
         <v>422</v>
       </c>
-      <c r="I41" s="36" t="s">
+      <c r="I41" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="J41" s="36" t="s">
+      <c r="J41" s="28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B42" s="35">
+    <row r="42" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B42" s="27">
         <v>2021</v>
       </c>
-      <c r="C42" s="33" t="s">
+      <c r="C42" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="33" t="s">
+      <c r="D42" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E42" s="33">
+      <c r="E42" s="25">
         <v>217</v>
       </c>
-      <c r="F42" s="33">
+      <c r="F42" s="25">
         <v>1607</v>
       </c>
-      <c r="G42" s="33">
+      <c r="G42" s="25">
         <v>23</v>
       </c>
-      <c r="H42" s="33">
+      <c r="H42" s="25">
         <v>197</v>
       </c>
-      <c r="I42" s="36" t="s">
+      <c r="I42" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="J42" s="36" t="s">
+      <c r="J42" s="28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B43" s="35">
+    <row r="43" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B43" s="27">
         <v>2021</v>
       </c>
-      <c r="C43" s="33" t="s">
+      <c r="C43" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D43" s="33" t="s">
+      <c r="D43" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E43" s="33">
+      <c r="E43" s="25">
         <v>216</v>
       </c>
-      <c r="F43" s="33">
+      <c r="F43" s="25">
         <v>1608</v>
       </c>
-      <c r="G43" s="33">
+      <c r="G43" s="25">
         <v>18</v>
       </c>
-      <c r="H43" s="33">
+      <c r="H43" s="25">
         <v>225</v>
       </c>
-      <c r="I43" s="36" t="s">
+      <c r="I43" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="J43" s="36" t="s">
+      <c r="J43" s="28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B44" s="35">
+    <row r="44" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B44" s="27">
         <v>2021</v>
       </c>
-      <c r="C44" s="33" t="s">
+      <c r="C44" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="33" t="s">
+      <c r="D44" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="33">
+      <c r="E44" s="25">
         <v>184</v>
       </c>
-      <c r="F44" s="33">
+      <c r="F44" s="25">
         <v>1039</v>
       </c>
-      <c r="G44" s="33">
+      <c r="G44" s="25">
         <v>38</v>
       </c>
-      <c r="H44" s="33">
+      <c r="H44" s="25">
         <v>392</v>
       </c>
-      <c r="I44" s="36" t="s">
+      <c r="I44" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="J44" s="36" t="s">
+      <c r="J44" s="28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B45" s="35">
+    <row r="45" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B45" s="27">
         <v>2021</v>
       </c>
-      <c r="C45" s="33" t="s">
+      <c r="C45" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D45" s="33" t="s">
+      <c r="D45" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E45" s="33">
+      <c r="E45" s="25">
         <v>101</v>
       </c>
-      <c r="F45" s="33">
+      <c r="F45" s="25">
         <v>534</v>
       </c>
-      <c r="G45" s="33">
+      <c r="G45" s="25">
         <v>23</v>
       </c>
-      <c r="H45" s="33">
+      <c r="H45" s="25">
         <v>207</v>
       </c>
-      <c r="I45" s="36" t="s">
+      <c r="I45" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="J45" s="36" t="s">
+      <c r="J45" s="28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="2:10" s="7" customFormat="1" ht="8.25">
-      <c r="B46" s="35">
+    <row r="46" spans="2:10" s="4" customFormat="1" ht="8.25">
+      <c r="B46" s="27">
         <v>2021</v>
       </c>
-      <c r="C46" s="33" t="s">
+      <c r="C46" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="33" t="s">
+      <c r="D46" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E46" s="33">
+      <c r="E46" s="25">
         <v>83</v>
       </c>
-      <c r="F46" s="33">
+      <c r="F46" s="25">
         <v>505</v>
       </c>
-      <c r="G46" s="33">
+      <c r="G46" s="25">
         <v>15</v>
       </c>
-      <c r="H46" s="33">
+      <c r="H46" s="25">
         <v>186</v>
       </c>
-      <c r="I46" s="36" t="s">
+      <c r="I46" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="J46" s="36" t="s">
+      <c r="J46" s="28" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="2:10" ht="8.25" customHeight="1"/>
     <row r="48" spans="2:10" ht="8.25" customHeight="1">
-      <c r="B48" s="19"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-    </row>
-    <row r="49" spans="1:13" s="21" customFormat="1" ht="8.25" customHeight="1">
-      <c r="B49" s="22" t="s">
+      <c r="B48" s="11"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+    </row>
+    <row r="49" spans="1:13" s="13" customFormat="1" ht="8.25" customHeight="1">
+      <c r="B49" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="24"/>
-      <c r="I49" s="24"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="23"/>
-    </row>
-    <row r="50" spans="1:13" s="21" customFormat="1" ht="8.25" customHeight="1">
-      <c r="B50" s="22" t="s">
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+    </row>
+    <row r="50" spans="1:13" s="13" customFormat="1" ht="8.25" customHeight="1">
+      <c r="B50" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="25"/>
-      <c r="I50" s="25"/>
-      <c r="J50" s="25"/>
-      <c r="K50" s="25"/>
-      <c r="L50" s="25"/>
-    </row>
-    <row r="51" spans="1:13" s="21" customFormat="1" ht="8.25" customHeight="1">
-      <c r="B51" s="22" t="s">
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+    </row>
+    <row r="51" spans="1:13" s="13" customFormat="1" ht="8.25" customHeight="1">
+      <c r="B51" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
-      <c r="J51" s="26"/>
-      <c r="K51" s="26"/>
-      <c r="L51" s="26"/>
-    </row>
-    <row r="52" spans="1:13" s="29" customFormat="1" ht="8.25" customHeight="1">
-      <c r="A52" s="27"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="28"/>
-      <c r="H52" s="28"/>
-      <c r="I52" s="28"/>
-      <c r="J52" s="28"/>
-      <c r="K52" s="27"/>
-      <c r="L52" s="27"/>
-      <c r="M52" s="27"/>
-    </row>
-    <row r="53" spans="1:13" s="29" customFormat="1" ht="8.25" customHeight="1">
-      <c r="B53" s="30" t="s">
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
+    </row>
+    <row r="52" spans="1:13" s="21" customFormat="1" ht="8.25" customHeight="1">
+      <c r="A52" s="19"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="19"/>
+      <c r="M52" s="19"/>
+    </row>
+    <row r="53" spans="1:13" s="21" customFormat="1" ht="8.25" customHeight="1">
+      <c r="B53" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="30"/>
-      <c r="H53" s="30"/>
-      <c r="I53" s="30"/>
-      <c r="J53" s="30"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
     </row>
     <row r="54" spans="1:13" ht="8.25" customHeight="1"/>
     <row r="55" spans="1:13" ht="8.25" customHeight="1">
-      <c r="B55" s="30" t="s">
+      <c r="B55" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
     </row>
     <row r="56" spans="1:13" ht="8.25" customHeight="1">
-      <c r="B56" s="30" t="s">
+      <c r="B56" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
     </row>
     <row r="57" spans="1:13" ht="8.25" customHeight="1">
-      <c r="B57" s="30" t="s">
+      <c r="B57" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
     </row>
     <row r="58" spans="1:13" ht="8.25" customHeight="1">
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C58" s="31"/>
-      <c r="D58" s="31"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>